<commit_message>
cópia de segurança para troca de equipamento
</commit_message>
<xml_diff>
--- a/Retorno do envio.xlsx
+++ b/Retorno do envio.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="209">
   <si>
     <t>CPF / CNPJ</t>
   </si>
@@ -37,31 +37,610 @@
     <t>STATUS EMAIL</t>
   </si>
   <si>
-    <t>55415865, 4254854445, 11982662870</t>
-  </si>
-  <si>
-    <t>43215432, 11951496374</t>
-  </si>
-  <si>
-    <t>23456789, 11981317092</t>
-  </si>
-  <si>
-    <t>sergio pj</t>
-  </si>
-  <si>
-    <t>Yasminzinha Mini</t>
-  </si>
-  <si>
-    <t>Rog gério</t>
-  </si>
-  <si>
-    <t>enviado, tel sem whats,enviado,</t>
-  </si>
-  <si>
-    <t>tel sem whats,tel sem whats</t>
-  </si>
-  <si>
-    <t>tel sem whats,enviado,</t>
+    <t>(11) 969491983,(11) 42448700,</t>
+  </si>
+  <si>
+    <t>(11) 982993320,,</t>
+  </si>
+  <si>
+    <t>(11) 999682960,,</t>
+  </si>
+  <si>
+    <t>(11) 997549740,(11) 41498271,(11) 974720124</t>
+  </si>
+  <si>
+    <t>(11) 945308870,(11) 47822196,</t>
+  </si>
+  <si>
+    <t>(11) 976752663,(11) 995532786,(11) 939099278</t>
+  </si>
+  <si>
+    <t>(11) 985777515,(11) 930007662,</t>
+  </si>
+  <si>
+    <t>(11) 988177700,(11) 43852186,(11) 951387648</t>
+  </si>
+  <si>
+    <t>(11) 973397381,,</t>
+  </si>
+  <si>
+    <t>(11) 958617596,,</t>
+  </si>
+  <si>
+    <t>(11) 965553427,,</t>
+  </si>
+  <si>
+    <t>(11) 967713546,(11) 41490379,</t>
+  </si>
+  <si>
+    <t>(11) 983762326,(11) 983762325,(11) 47826210</t>
+  </si>
+  <si>
+    <t>(11) 951370259,(11) 42442833,</t>
+  </si>
+  <si>
+    <t>(11) 934207546,(11) 42031840,</t>
+  </si>
+  <si>
+    <t>(11) 58258646,,</t>
+  </si>
+  <si>
+    <t>(11) 966102897,(11) 947848687,(11) 47853500</t>
+  </si>
+  <si>
+    <t>(11) 970934712,(11) 41498144,</t>
+  </si>
+  <si>
+    <t>(11) 965210814,,</t>
+  </si>
+  <si>
+    <t>(11) 955571823,(11) 962612810,(11) 960281550</t>
+  </si>
+  <si>
+    <t>(84) 991354150,,</t>
+  </si>
+  <si>
+    <t>(11) 996834257,(11) 961661190,(11) 47834281</t>
+  </si>
+  <si>
+    <t>(11) 981126455,,</t>
+  </si>
+  <si>
+    <t>(11) 954866838,(11) 42034099,(11) 986978815</t>
+  </si>
+  <si>
+    <t>(11) 912011131,(11) 979918343,</t>
+  </si>
+  <si>
+    <t>(11) 960892915,,</t>
+  </si>
+  <si>
+    <t>(11) 986038141,(11) 42441958,</t>
+  </si>
+  <si>
+    <t>(11) 43851140,(11) 986058479,</t>
+  </si>
+  <si>
+    <t>(11) 976448255,(11) 47826822,(11) 987888099</t>
+  </si>
+  <si>
+    <t>(11) 969240746,,</t>
+  </si>
+  <si>
+    <t>(11) 953676149,(11) 987011558,</t>
+  </si>
+  <si>
+    <t>(11) 976921552,(11) 47838395,</t>
+  </si>
+  <si>
+    <t>(11) 982396539,(11) 41491409,</t>
+  </si>
+  <si>
+    <t>(11) 945538252,(11) 945438252,(11) 47820787</t>
+  </si>
+  <si>
+    <t>(11) 945400927,,</t>
+  </si>
+  <si>
+    <t>(11) 985654601,,</t>
+  </si>
+  <si>
+    <t>(11) 977977120,(11) 47826238,</t>
+  </si>
+  <si>
+    <t>(11) 984548419,,</t>
+  </si>
+  <si>
+    <t>(11) 982675298,,</t>
+  </si>
+  <si>
+    <t>(13) 991626038,(13) 978145698,(13) 32991290</t>
+  </si>
+  <si>
+    <t>(11) 952988908,(11) 973622146,(11) 25475222</t>
+  </si>
+  <si>
+    <t>(11) 968506765,,</t>
+  </si>
+  <si>
+    <t>(11) 69528419,(11) 969528419,</t>
+  </si>
+  <si>
+    <t>(11) 964368365,,</t>
+  </si>
+  <si>
+    <t>(11) 987955274,(11) 47825805,</t>
+  </si>
+  <si>
+    <t>(11) 911312330,(11) 42441653,</t>
+  </si>
+  <si>
+    <t>(11) 997043724,(11) 970437241,</t>
+  </si>
+  <si>
+    <t>(11) 985005705,,</t>
+  </si>
+  <si>
+    <t>,(11) 947691355,</t>
+  </si>
+  <si>
+    <t>(11) 957502709,,</t>
+  </si>
+  <si>
+    <t>(11) 42032084,(11) 952998900,</t>
+  </si>
+  <si>
+    <t>(11) 962990902,(11) 45539229,</t>
+  </si>
+  <si>
+    <t>(11) 953396028,,</t>
+  </si>
+  <si>
+    <t>(11) 972534691,(11) 47810141,</t>
+  </si>
+  <si>
+    <t>(11) 947320102,(11) 994174910,(11) 947175918</t>
+  </si>
+  <si>
+    <t>(11) 972283164,(11) 41493106,</t>
+  </si>
+  <si>
+    <t>(11) 946032876,(11) 47825094,(11) 952077064</t>
+  </si>
+  <si>
+    <t>JOSELUIZMENDESDACOSTA@GMAILCOM</t>
+  </si>
+  <si>
+    <t>DIOGOMALINHA@BOLCOMBR</t>
+  </si>
+  <si>
+    <t>JORGE2037@TERRACOMBR</t>
+  </si>
+  <si>
+    <t>LUIZPINA1956@GMAILCOM</t>
+  </si>
+  <si>
+    <t>joseraididesousa@gmailcom</t>
+  </si>
+  <si>
+    <t>CELSOTADEUSILVA1@GMAILCOM</t>
+  </si>
+  <si>
+    <t>WMPERSONAL@OUTLOOKCOM</t>
+  </si>
+  <si>
+    <t>ALVESTSILVA227@GMAILCOM</t>
+  </si>
+  <si>
+    <t>GERALDOANTONIOPEDROSA566@GMAILCOM</t>
+  </si>
+  <si>
+    <t>KARINEALVES86@YAHOOCOM</t>
+  </si>
+  <si>
+    <t>BIRARIOLA@HOTMAILCOM</t>
+  </si>
+  <si>
+    <t>NAOTEM@NAOTEMCOMBR</t>
+  </si>
+  <si>
+    <t>ADEAQUINO@IGCOMBR</t>
+  </si>
+  <si>
+    <t>LEONIDASSILVAGONCALVES@GMAILCOM</t>
+  </si>
+  <si>
+    <t>AGNALDONASCIMENTOGUIGUI52@GMAILCOM</t>
+  </si>
+  <si>
+    <t>FRANCISCOFERNANDES0421@GMAILCOM</t>
+  </si>
+  <si>
+    <t>DEMAZITEOLOPES@HOTMAILCOM</t>
+  </si>
+  <si>
+    <t>ANTONIOZARREF@GMAILCOM</t>
+  </si>
+  <si>
+    <t>JACQUELINELOPES729@GMAILCOM</t>
+  </si>
+  <si>
+    <t>VILMA_GALVAO@HOTMAILCOM</t>
+  </si>
+  <si>
+    <t>JOSEALVESLIMA42@GMAILCOM</t>
+  </si>
+  <si>
+    <t>ANTONIOREIS0804@GMAILCOM</t>
+  </si>
+  <si>
+    <t>OLIVEIRAJORGETEL@GMAILCOM</t>
+  </si>
+  <si>
+    <t>CAMILAHS@TERRACOMBR</t>
+  </si>
+  <si>
+    <t>LANACORREIA@IGCOMBR</t>
+  </si>
+  <si>
+    <t>EDSONJOSEARRUDA18@GMAILCOM</t>
+  </si>
+  <si>
+    <t>LUIZLETRISTA09@GMAILCOM</t>
+  </si>
+  <si>
+    <t>IRENECARMOMARTINS@GMAILCOM</t>
+  </si>
+  <si>
+    <t>MARLENEMELOPEREIRA@YAHOOCOMBR</t>
+  </si>
+  <si>
+    <t>ANTONIODOMINGO6619@GMAILCOM</t>
+  </si>
+  <si>
+    <t>msedson50@gmailcom</t>
+  </si>
+  <si>
+    <t>JOICEGAMP@YAHOOCOM</t>
+  </si>
+  <si>
+    <t>LIVIA_MOLINA@IGCOMBR</t>
+  </si>
+  <si>
+    <t>GUSMANPEDROSA02@GMAILCOM</t>
+  </si>
+  <si>
+    <t>HUGOHIGOSKTAG@GMAILCOM</t>
+  </si>
+  <si>
+    <t>RENATO554@LIVECOM</t>
+  </si>
+  <si>
+    <t>MAMONTEIRO2000@HOTMAILCOM</t>
+  </si>
+  <si>
+    <t>AVARECONSTRUCAO@UOLCOMBR</t>
+  </si>
+  <si>
+    <t>JOVELINOSANTOS@YAHOOCOMBR</t>
+  </si>
+  <si>
+    <t>ARCONTSP@HOTMAILCOM</t>
+  </si>
+  <si>
+    <t>GERINALDOMARINHO@TERRACOMBR</t>
+  </si>
+  <si>
+    <t>FRANCISCOFRANKLIN941@GMAILCOM</t>
+  </si>
+  <si>
+    <t>BIANCANICOLY14@GMAILCOM</t>
+  </si>
+  <si>
+    <t>FERNANDASYM65@GMAILCOM</t>
+  </si>
+  <si>
+    <t>LUANAOLIVEIRA01@GLOBOCOM</t>
+  </si>
+  <si>
+    <t>ALINEJUNIOR17@GMAILCOM</t>
+  </si>
+  <si>
+    <t>APARECIDO_2142@GMAILCOM</t>
+  </si>
+  <si>
+    <t>JACQUE_ROMAO@LIVECOM</t>
+  </si>
+  <si>
+    <t>99595796891JOSE LUIZ MENDES DA COSTA</t>
+  </si>
+  <si>
+    <t>99553406815JOAO ANSELMO FILHO</t>
+  </si>
+  <si>
+    <t>95301887815JORGE FERNANDES</t>
+  </si>
+  <si>
+    <t>94383413820LUIZ ANTONIO DE SOUZA PINA</t>
+  </si>
+  <si>
+    <t>94369836891JOSE RAIDI DE SOUSA</t>
+  </si>
+  <si>
+    <t>93860277804CELSO TADEU DA SILVA</t>
+  </si>
+  <si>
+    <t>93817983891FRANCISCO PAULO DOS SANTOS</t>
+  </si>
+  <si>
+    <t>93719647820MANUEL MARTINS DA SILVA</t>
+  </si>
+  <si>
+    <t>93293690815ANTONIO ALVES DA SILVA</t>
+  </si>
+  <si>
+    <t>91544742800JOSE GERALDO ANTONIO PEDROSA</t>
+  </si>
+  <si>
+    <t>91540232891ADAO GONCALVES DE OLIVEIRA</t>
+  </si>
+  <si>
+    <t>91392985820LUIZ CARLOS SOARES</t>
+  </si>
+  <si>
+    <t>89947827887JOSE ALVES DOS SANTOS</t>
+  </si>
+  <si>
+    <t>89258690800ADEMAR JOSE DE AQUINO</t>
+  </si>
+  <si>
+    <t>88126056800LEONIDAS DA SILVA GONCALVES</t>
+  </si>
+  <si>
+    <t>87667444820JOAO LUIS LEONEL</t>
+  </si>
+  <si>
+    <t>85711616820AGNALDO OLIVEIRA DO NASCIMENTO</t>
+  </si>
+  <si>
+    <t>85442330825FRANCISCO FERNANDES DE SOUZA</t>
+  </si>
+  <si>
+    <t>84631082887ADEMAR RABELO LOPES</t>
+  </si>
+  <si>
+    <t>84614447872LIDIA ULIACH NARDES</t>
+  </si>
+  <si>
+    <t>83693688834ANTONIO FERRAZ</t>
+  </si>
+  <si>
+    <t>81829248804ANTONIO GOMES SODRE</t>
+  </si>
+  <si>
+    <t>81293615668DENISE LOPES FARIAS</t>
+  </si>
+  <si>
+    <t>81219288853IRINEU VIANA</t>
+  </si>
+  <si>
+    <t>81103018868JOSE ALVES DE LIMA</t>
+  </si>
+  <si>
+    <t>80517323834ANTONIO DE OLIVEIRA REIS</t>
+  </si>
+  <si>
+    <t>79149480804JORGE TEODORO DE OLIVEIRA</t>
+  </si>
+  <si>
+    <t>76920860872JOSE RAIMUNDO FERREIRA DE SOUZA</t>
+  </si>
+  <si>
+    <t>76660885820LINO DA SILVA PIMENTA</t>
+  </si>
+  <si>
+    <t>76186229815EDSON JOSE ARRUDA</t>
+  </si>
+  <si>
+    <t>75773651815MARIA DA CONCEICAO CUPERTINO SILVA</t>
+  </si>
+  <si>
+    <t>75470080897IRENE DO CARMO MARTINS GOMES</t>
+  </si>
+  <si>
+    <t>71721576649EVA DE SOUSA PEREIRA</t>
+  </si>
+  <si>
+    <t>69893390800ANTONIO DOMINGOS DA SILVA</t>
+  </si>
+  <si>
+    <t>69651841834EDSON MIRANDA SILVA</t>
+  </si>
+  <si>
+    <t>69515387868ANTONIO FELICIANO DE OLIVEIRA</t>
+  </si>
+  <si>
+    <t>69291322849LIVIA MOLINA BERNARDINO</t>
+  </si>
+  <si>
+    <t>68581106820CARLOS ALBERTO GUSMAN PEDROSA</t>
+  </si>
+  <si>
+    <t>67766064804JOAO FRANCISCO MARTINS FILHO</t>
+  </si>
+  <si>
+    <t>66347289849EVERALDO CLARO DA COSTA</t>
+  </si>
+  <si>
+    <t>66297974853BEIJAMIM LOPES DE ARAUJO</t>
+  </si>
+  <si>
+    <t>64295516872ELISEU DE SOUZA SANTOS</t>
+  </si>
+  <si>
+    <t>62933639815JOVELINO JOSE DOS SANTOS</t>
+  </si>
+  <si>
+    <t>61376558734AFONSO JOAO DE SANTANA</t>
+  </si>
+  <si>
+    <t>53587499853GERINALDO MARINHO</t>
+  </si>
+  <si>
+    <t>52075257868FRANCISCO FRANKLIN ROCHA</t>
+  </si>
+  <si>
+    <t>48508519400ALUIZIO MAURO DA SILVA</t>
+  </si>
+  <si>
+    <t>47387467587EDNALDO AMPARO DOS SANTOS</t>
+  </si>
+  <si>
+    <t>45537605848BIANCA GAVIAO DANIEL</t>
+  </si>
+  <si>
+    <t>44375662700JOSE JOSIVAL DE OLIVEIRA NOBREGA</t>
+  </si>
+  <si>
+    <t>42480868834LAERCIO DE OLIVEIRA</t>
+  </si>
+  <si>
+    <t>41155205820FERNANDA DE SOUZA ANDRADE</t>
+  </si>
+  <si>
+    <t>40660111870MARIA DE LOURDES BARBOSA DOS SANTOS</t>
+  </si>
+  <si>
+    <t>40558261841LUANA DE OLIVEIRA SILVA</t>
+  </si>
+  <si>
+    <t>37396806879ALINE CRISTINA PEREIRA</t>
+  </si>
+  <si>
+    <t>36956279991APARECIDO RODRIGUES DA SILVA</t>
+  </si>
+  <si>
+    <t>36658997888JACQUELINE DE ASSIS ROMAO CAVALHEIRO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JOSE </t>
+  </si>
+  <si>
+    <t xml:space="preserve">JOAO </t>
+  </si>
+  <si>
+    <t xml:space="preserve">JORGE </t>
+  </si>
+  <si>
+    <t xml:space="preserve">LUIZ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CELSO </t>
+  </si>
+  <si>
+    <t xml:space="preserve">FRANCISCO </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MANUEL </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANTONIO </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADAO </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADEMAR </t>
+  </si>
+  <si>
+    <t xml:space="preserve">LEONIDAS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AGNALDO </t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIDIA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DENISE </t>
+  </si>
+  <si>
+    <t xml:space="preserve">IRINEU </t>
+  </si>
+  <si>
+    <t xml:space="preserve">LINO </t>
+  </si>
+  <si>
+    <t xml:space="preserve">EDSON </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MARIA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">IRENE </t>
+  </si>
+  <si>
+    <t xml:space="preserve">EVA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIVIA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CARLOS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">EVERALDO </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BEIJAMIM </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ELISEU </t>
+  </si>
+  <si>
+    <t xml:space="preserve">JOVELINO </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AFONSO </t>
+  </si>
+  <si>
+    <t xml:space="preserve">GERINALDO </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALUIZIO </t>
+  </si>
+  <si>
+    <t xml:space="preserve">EDNALDO </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BIANCA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">LAERCIO </t>
+  </si>
+  <si>
+    <t xml:space="preserve">FERNANDA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">LUANA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALINE </t>
+  </si>
+  <si>
+    <t xml:space="preserve">APARECIDO </t>
+  </si>
+  <si>
+    <t xml:space="preserve">JACQUELINE </t>
+  </si>
+  <si>
+    <t>tel sem whats,tel sem whats,</t>
+  </si>
+  <si>
+    <t>tel sem whats,</t>
+  </si>
+  <si>
+    <t>tel sem whats,tel sem whats,tel sem whats,</t>
   </si>
 </sst>
 </file>
@@ -419,7 +998,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -449,36 +1028,987 @@
       </c>
     </row>
     <row r="2" spans="1:7">
+      <c r="A2">
+        <v>99595796891</v>
+      </c>
       <c r="B2" t="s">
         <v>7</v>
       </c>
+      <c r="C2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" t="s">
+        <v>112</v>
+      </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>169</v>
       </c>
       <c r="F2" t="s">
-        <v>13</v>
+        <v>206</v>
       </c>
     </row>
     <row r="3" spans="1:7">
+      <c r="A3">
+        <v>99553406815</v>
+      </c>
       <c r="B3" t="s">
         <v>8</v>
       </c>
+      <c r="C3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" t="s">
+        <v>113</v>
+      </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>170</v>
       </c>
       <c r="F3" t="s">
-        <v>14</v>
+        <v>207</v>
       </c>
     </row>
     <row r="4" spans="1:7">
+      <c r="A4">
+        <v>95301887815</v>
+      </c>
       <c r="B4" t="s">
         <v>9</v>
       </c>
+      <c r="C4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D4" t="s">
+        <v>114</v>
+      </c>
       <c r="E4" t="s">
+        <v>171</v>
+      </c>
+      <c r="F4" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5">
+        <v>94383413820</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D5" t="s">
+        <v>115</v>
+      </c>
+      <c r="E5" t="s">
+        <v>172</v>
+      </c>
+      <c r="F5" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6">
+        <v>94369836891</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D6" t="s">
+        <v>116</v>
+      </c>
+      <c r="E6" t="s">
+        <v>169</v>
+      </c>
+      <c r="F6" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7">
+        <v>93860277804</v>
+      </c>
+      <c r="B7" t="s">
         <v>12</v>
       </c>
-      <c r="F4" t="s">
+      <c r="C7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D7" t="s">
+        <v>117</v>
+      </c>
+      <c r="E7" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8">
+        <v>93817983891</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8" t="s">
+        <v>118</v>
+      </c>
+      <c r="E8" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9">
+        <v>93719647820</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>70</v>
+      </c>
+      <c r="D9" t="s">
+        <v>119</v>
+      </c>
+      <c r="E9" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10">
+        <v>93293690815</v>
+      </c>
+      <c r="B10" t="s">
         <v>15</v>
+      </c>
+      <c r="C10" t="s">
+        <v>71</v>
+      </c>
+      <c r="D10" t="s">
+        <v>120</v>
+      </c>
+      <c r="E10" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11">
+        <v>91544742800</v>
+      </c>
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" t="s">
+        <v>72</v>
+      </c>
+      <c r="D11" t="s">
+        <v>121</v>
+      </c>
+      <c r="E11" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12">
+        <v>91540232891</v>
+      </c>
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" t="s">
+        <v>73</v>
+      </c>
+      <c r="D12" t="s">
+        <v>122</v>
+      </c>
+      <c r="E12" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13">
+        <v>91392985820</v>
+      </c>
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" t="s">
+        <v>74</v>
+      </c>
+      <c r="D13" t="s">
+        <v>123</v>
+      </c>
+      <c r="E13" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14">
+        <v>89947827887</v>
+      </c>
+      <c r="B14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" t="s">
+        <v>75</v>
+      </c>
+      <c r="D14" t="s">
+        <v>124</v>
+      </c>
+      <c r="E14" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15">
+        <v>89258690800</v>
+      </c>
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" t="s">
+        <v>76</v>
+      </c>
+      <c r="D15" t="s">
+        <v>125</v>
+      </c>
+      <c r="E15" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16">
+        <v>88126056800</v>
+      </c>
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" t="s">
+        <v>77</v>
+      </c>
+      <c r="D16" t="s">
+        <v>126</v>
+      </c>
+      <c r="E16" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17">
+        <v>87667444820</v>
+      </c>
+      <c r="B17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17" t="s">
+        <v>127</v>
+      </c>
+      <c r="E17" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18">
+        <v>85711616820</v>
+      </c>
+      <c r="B18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" t="s">
+        <v>78</v>
+      </c>
+      <c r="D18" t="s">
+        <v>128</v>
+      </c>
+      <c r="E18" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19">
+        <v>85442330825</v>
+      </c>
+      <c r="B19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" t="s">
+        <v>79</v>
+      </c>
+      <c r="D19" t="s">
+        <v>129</v>
+      </c>
+      <c r="E19" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20">
+        <v>84631082887</v>
+      </c>
+      <c r="B20" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" t="s">
+        <v>80</v>
+      </c>
+      <c r="D20" t="s">
+        <v>130</v>
+      </c>
+      <c r="E20" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21">
+        <v>84614447872</v>
+      </c>
+      <c r="B21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21" t="s">
+        <v>131</v>
+      </c>
+      <c r="E21" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22">
+        <v>83693688834</v>
+      </c>
+      <c r="B22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" t="s">
+        <v>81</v>
+      </c>
+      <c r="D22" t="s">
+        <v>132</v>
+      </c>
+      <c r="E22" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23">
+        <v>81829248804</v>
+      </c>
+      <c r="B23" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23" t="s">
+        <v>133</v>
+      </c>
+      <c r="E23" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24">
+        <v>81293615668</v>
+      </c>
+      <c r="B24" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" t="s">
+        <v>82</v>
+      </c>
+      <c r="D24" t="s">
+        <v>134</v>
+      </c>
+      <c r="E24" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25">
+        <v>81219288853</v>
+      </c>
+      <c r="B25" t="s">
+        <v>30</v>
+      </c>
+      <c r="C25" t="s">
+        <v>83</v>
+      </c>
+      <c r="D25" t="s">
+        <v>135</v>
+      </c>
+      <c r="E25" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26">
+        <v>81103018868</v>
+      </c>
+      <c r="B26" t="s">
+        <v>31</v>
+      </c>
+      <c r="C26" t="s">
+        <v>84</v>
+      </c>
+      <c r="D26" t="s">
+        <v>136</v>
+      </c>
+      <c r="E26" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27">
+        <v>80517323834</v>
+      </c>
+      <c r="B27" t="s">
+        <v>32</v>
+      </c>
+      <c r="C27" t="s">
+        <v>85</v>
+      </c>
+      <c r="D27" t="s">
+        <v>137</v>
+      </c>
+      <c r="E27" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28">
+        <v>79149480804</v>
+      </c>
+      <c r="B28" t="s">
+        <v>33</v>
+      </c>
+      <c r="C28" t="s">
+        <v>86</v>
+      </c>
+      <c r="D28" t="s">
+        <v>138</v>
+      </c>
+      <c r="E28" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29">
+        <v>76920860872</v>
+      </c>
+      <c r="B29" t="s">
+        <v>34</v>
+      </c>
+      <c r="C29" t="s">
+        <v>87</v>
+      </c>
+      <c r="D29" t="s">
+        <v>139</v>
+      </c>
+      <c r="E29" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30">
+        <v>76660885820</v>
+      </c>
+      <c r="B30" t="s">
+        <v>35</v>
+      </c>
+      <c r="C30" t="s">
+        <v>88</v>
+      </c>
+      <c r="D30" t="s">
+        <v>140</v>
+      </c>
+      <c r="E30" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31">
+        <v>76186229815</v>
+      </c>
+      <c r="B31" t="s">
+        <v>36</v>
+      </c>
+      <c r="C31" t="s">
+        <v>89</v>
+      </c>
+      <c r="D31" t="s">
+        <v>141</v>
+      </c>
+      <c r="E31" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32">
+        <v>75773651815</v>
+      </c>
+      <c r="B32" t="s">
+        <v>37</v>
+      </c>
+      <c r="C32" t="s">
+        <v>90</v>
+      </c>
+      <c r="D32" t="s">
+        <v>142</v>
+      </c>
+      <c r="E32" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33">
+        <v>75470080897</v>
+      </c>
+      <c r="B33" t="s">
+        <v>38</v>
+      </c>
+      <c r="C33" t="s">
+        <v>91</v>
+      </c>
+      <c r="D33" t="s">
+        <v>143</v>
+      </c>
+      <c r="E33" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34">
+        <v>71721576649</v>
+      </c>
+      <c r="B34" t="s">
+        <v>39</v>
+      </c>
+      <c r="C34" t="s">
+        <v>92</v>
+      </c>
+      <c r="D34" t="s">
+        <v>144</v>
+      </c>
+      <c r="E34" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35">
+        <v>69893390800</v>
+      </c>
+      <c r="B35" t="s">
+        <v>40</v>
+      </c>
+      <c r="C35" t="s">
+        <v>93</v>
+      </c>
+      <c r="D35" t="s">
+        <v>145</v>
+      </c>
+      <c r="E35" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36">
+        <v>69651841834</v>
+      </c>
+      <c r="B36" t="s">
+        <v>41</v>
+      </c>
+      <c r="C36" t="s">
+        <v>94</v>
+      </c>
+      <c r="D36" t="s">
+        <v>146</v>
+      </c>
+      <c r="E36" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37">
+        <v>69515387868</v>
+      </c>
+      <c r="B37" t="s">
+        <v>42</v>
+      </c>
+      <c r="C37" t="s">
+        <v>95</v>
+      </c>
+      <c r="D37" t="s">
+        <v>147</v>
+      </c>
+      <c r="E37" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38">
+        <v>69291322849</v>
+      </c>
+      <c r="B38" t="s">
+        <v>43</v>
+      </c>
+      <c r="C38" t="s">
+        <v>96</v>
+      </c>
+      <c r="D38" t="s">
+        <v>148</v>
+      </c>
+      <c r="E38" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39">
+        <v>68581106820</v>
+      </c>
+      <c r="B39" t="s">
+        <v>44</v>
+      </c>
+      <c r="C39" t="s">
+        <v>97</v>
+      </c>
+      <c r="D39" t="s">
+        <v>149</v>
+      </c>
+      <c r="E39" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40">
+        <v>67766064804</v>
+      </c>
+      <c r="B40" t="s">
+        <v>45</v>
+      </c>
+      <c r="C40" t="s">
+        <v>98</v>
+      </c>
+      <c r="D40" t="s">
+        <v>150</v>
+      </c>
+      <c r="E40" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41">
+        <v>66347289849</v>
+      </c>
+      <c r="B41" t="s">
+        <v>46</v>
+      </c>
+      <c r="C41" t="s">
+        <v>99</v>
+      </c>
+      <c r="D41" t="s">
+        <v>151</v>
+      </c>
+      <c r="E41" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42">
+        <v>66297974853</v>
+      </c>
+      <c r="B42" t="s">
+        <v>47</v>
+      </c>
+      <c r="C42" t="s">
+        <v>100</v>
+      </c>
+      <c r="D42" t="s">
+        <v>152</v>
+      </c>
+      <c r="E42" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43">
+        <v>64295516872</v>
+      </c>
+      <c r="B43" t="s">
+        <v>48</v>
+      </c>
+      <c r="C43" t="s">
+        <v>101</v>
+      </c>
+      <c r="D43" t="s">
+        <v>153</v>
+      </c>
+      <c r="E43" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44">
+        <v>62933639815</v>
+      </c>
+      <c r="B44" t="s">
+        <v>49</v>
+      </c>
+      <c r="C44" t="s">
+        <v>102</v>
+      </c>
+      <c r="D44" t="s">
+        <v>154</v>
+      </c>
+      <c r="E44" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45">
+        <v>61376558734</v>
+      </c>
+      <c r="B45" t="s">
+        <v>50</v>
+      </c>
+      <c r="C45" t="s">
+        <v>103</v>
+      </c>
+      <c r="D45" t="s">
+        <v>155</v>
+      </c>
+      <c r="E45" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46">
+        <v>53587499853</v>
+      </c>
+      <c r="B46" t="s">
+        <v>51</v>
+      </c>
+      <c r="C46" t="s">
+        <v>104</v>
+      </c>
+      <c r="D46" t="s">
+        <v>156</v>
+      </c>
+      <c r="E46" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47">
+        <v>52075257868</v>
+      </c>
+      <c r="B47" t="s">
+        <v>52</v>
+      </c>
+      <c r="C47" t="s">
+        <v>105</v>
+      </c>
+      <c r="D47" t="s">
+        <v>157</v>
+      </c>
+      <c r="E47" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48">
+        <v>48508519400</v>
+      </c>
+      <c r="B48" t="s">
+        <v>53</v>
+      </c>
+      <c r="C48">
+        <v>0</v>
+      </c>
+      <c r="D48" t="s">
+        <v>158</v>
+      </c>
+      <c r="E48" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49">
+        <v>47387467587</v>
+      </c>
+      <c r="B49" t="s">
+        <v>54</v>
+      </c>
+      <c r="C49">
+        <v>0</v>
+      </c>
+      <c r="D49" t="s">
+        <v>159</v>
+      </c>
+      <c r="E49" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50">
+        <v>45537605848</v>
+      </c>
+      <c r="B50" t="s">
+        <v>55</v>
+      </c>
+      <c r="C50" t="s">
+        <v>106</v>
+      </c>
+      <c r="D50" t="s">
+        <v>160</v>
+      </c>
+      <c r="E50" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51">
+        <v>44375662700</v>
+      </c>
+      <c r="B51" t="s">
+        <v>56</v>
+      </c>
+      <c r="C51">
+        <v>0</v>
+      </c>
+      <c r="D51" t="s">
+        <v>161</v>
+      </c>
+      <c r="E51" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52">
+        <v>42480868834</v>
+      </c>
+      <c r="B52" t="s">
+        <v>57</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="D52" t="s">
+        <v>162</v>
+      </c>
+      <c r="E52" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53">
+        <v>41155205820</v>
+      </c>
+      <c r="B53" t="s">
+        <v>58</v>
+      </c>
+      <c r="C53" t="s">
+        <v>107</v>
+      </c>
+      <c r="D53" t="s">
+        <v>163</v>
+      </c>
+      <c r="E53" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54">
+        <v>40660111870</v>
+      </c>
+      <c r="B54" t="s">
+        <v>59</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
+      </c>
+      <c r="D54" t="s">
+        <v>164</v>
+      </c>
+      <c r="E54" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55">
+        <v>40558261841</v>
+      </c>
+      <c r="B55" t="s">
+        <v>60</v>
+      </c>
+      <c r="C55" t="s">
+        <v>108</v>
+      </c>
+      <c r="D55" t="s">
+        <v>165</v>
+      </c>
+      <c r="E55" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56">
+        <v>37396806879</v>
+      </c>
+      <c r="B56" t="s">
+        <v>61</v>
+      </c>
+      <c r="C56" t="s">
+        <v>109</v>
+      </c>
+      <c r="D56" t="s">
+        <v>166</v>
+      </c>
+      <c r="E56" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57">
+        <v>36956279991</v>
+      </c>
+      <c r="B57" t="s">
+        <v>62</v>
+      </c>
+      <c r="C57" t="s">
+        <v>110</v>
+      </c>
+      <c r="D57" t="s">
+        <v>167</v>
+      </c>
+      <c r="E57" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58">
+        <v>36658997888</v>
+      </c>
+      <c r="B58" t="s">
+        <v>63</v>
+      </c>
+      <c r="C58" t="s">
+        <v>111</v>
+      </c>
+      <c r="D58" t="s">
+        <v>168</v>
+      </c>
+      <c r="E58" t="s">
+        <v>205</v>
       </c>
     </row>
   </sheetData>

</xml_diff>